<commit_message>
update regiester table documents
</commit_message>
<xml_diff>
--- a/I2C-master/documentation/registers.xlsx
+++ b/I2C-master/documentation/registers.xlsx
@@ -340,15 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -360,9 +351,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,15 +366,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,21 +728,21 @@
       <c r="K4" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6">
         <v>7</v>
@@ -771,7 +771,7 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -804,7 +804,7 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
@@ -835,7 +835,7 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -899,7 +899,7 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="6" t="s">
         <v>3</v>
       </c>
@@ -930,7 +930,7 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="6" t="s">
         <v>2</v>
       </c>
@@ -967,22 +967,22 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
       <c r="L15" s="1"/>
       <c r="N15" s="4" t="s">
         <v>22</v>
@@ -992,20 +992,20 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="1"/>
       <c r="N16" s="5" t="s">
         <v>23</v>
@@ -1015,20 +1015,20 @@
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="D17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
       <c r="L17" s="2"/>
       <c r="N17" s="5" t="s">
         <v>19</v>
@@ -1038,60 +1038,60 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="D19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1108,7 +1108,7 @@
       <c r="M21" s="7"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="18" t="s">
         <v>58</v>
       </c>
       <c r="I22" s="8"/>
@@ -1125,7 +1125,7 @@
       <c r="M22" s="7"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="6" t="s">
         <v>2</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1148,57 +1148,57 @@
       <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+      <c r="E26" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1207,57 +1207,57 @@
       <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="E29" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="8"/>
@@ -1272,12 +1272,12 @@
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="18" t="s">
         <v>58</v>
       </c>
       <c r="H31" s="8"/>
@@ -1287,7 +1287,7 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1300,7 +1300,7 @@
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="8"/>
@@ -1315,12 +1315,12 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="18" t="s">
         <v>58</v>
       </c>
       <c r="H34" s="8"/>
@@ -1330,7 +1330,7 @@
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -1344,6 +1344,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="E24:K24"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="E27:K27"/>
+    <mergeCell ref="E28:K28"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B33:B35"/>
@@ -1360,12 +1366,6 @@
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="D18:K18"/>
-    <mergeCell ref="E24:K24"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E27:K27"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="E29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1425,7 @@
       <c r="I5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1438,21 +1438,21 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N7" s="18"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" s="10"/>
@@ -1483,16 +1483,16 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="10" t="s">
@@ -1515,14 +1515,14 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D11" s="11"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -1545,14 +1545,14 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D12" s="11"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="10" t="s">
@@ -1575,7 +1575,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="25" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -1584,7 +1584,7 @@
       <c r="F13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="13" t="s">
         <v>27</v>
       </c>
       <c r="H13" s="10" t="s">
@@ -1605,25 +1605,25 @@
       <c r="M13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="Q13" s="25"/>
+      <c r="Q13" s="29"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="25" t="s">
+      <c r="S13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="25"/>
+      <c r="T13" s="29"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D14" s="11"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="10" t="s">
@@ -1644,29 +1644,29 @@
       <c r="M14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="21">
         <v>1</v>
       </c>
-      <c r="Q14" s="27" t="s">
+      <c r="Q14" s="22" t="s">
         <v>13</v>
       </c>
       <c r="R14" s="1"/>
-      <c r="S14" s="26">
+      <c r="S14" s="21">
         <v>1</v>
       </c>
-      <c r="T14" s="28" t="s">
+      <c r="T14" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D15" s="11"/>
+      <c r="D15" s="25"/>
       <c r="E15" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -1687,200 +1687,200 @@
       <c r="M15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="26">
+      <c r="P15" s="21">
         <v>2</v>
       </c>
-      <c r="Q15" s="27" t="s">
+      <c r="Q15" s="22" t="s">
         <v>14</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="26">
+      <c r="S15" s="21">
         <v>2</v>
       </c>
-      <c r="T15" s="27" t="s">
+      <c r="T15" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="P16" s="26">
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="P16" s="21">
         <v>3</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="Q16" s="22" t="s">
         <v>15</v>
       </c>
       <c r="R16" s="1"/>
-      <c r="S16" s="26">
+      <c r="S16" s="21">
         <v>3</v>
       </c>
-      <c r="T16" s="27" t="s">
+      <c r="T16" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D17" s="11"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="P17" s="26">
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="P17" s="21">
         <v>4</v>
       </c>
-      <c r="Q17" s="27" t="s">
+      <c r="Q17" s="22" t="s">
         <v>16</v>
       </c>
       <c r="R17" s="1"/>
-      <c r="S17" s="26">
+      <c r="S17" s="21">
         <v>4</v>
       </c>
-      <c r="T17" s="27" t="s">
+      <c r="T17" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D18" s="11"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="P18" s="26">
+      <c r="F18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="P18" s="21">
         <v>5</v>
       </c>
-      <c r="Q18" s="27" t="s">
+      <c r="Q18" s="22" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="26">
+      <c r="S18" s="21">
         <v>5</v>
       </c>
-      <c r="T18" s="28" t="s">
+      <c r="T18" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="25" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="P19" s="26">
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="P19" s="21">
         <v>6</v>
       </c>
-      <c r="Q19" s="27" t="s">
+      <c r="Q19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="26">
+      <c r="S19" s="21">
         <v>6</v>
       </c>
-      <c r="T19" s="27" t="s">
+      <c r="T19" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D20" s="11"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="P20" s="26">
+      <c r="F20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="P20" s="21">
         <v>7</v>
       </c>
-      <c r="Q20" s="27" t="s">
+      <c r="Q20" s="22" t="s">
         <v>31</v>
       </c>
       <c r="R20" s="1"/>
-      <c r="S20" s="26">
+      <c r="S20" s="21">
         <v>7</v>
       </c>
-      <c r="T20" s="27" t="s">
+      <c r="T20" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D21" s="11"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="P21" s="26">
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="P21" s="21">
         <v>8</v>
       </c>
-      <c r="Q21" s="27" t="s">
+      <c r="Q21" s="22" t="s">
         <v>35</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="26">
+      <c r="S21" s="21">
         <v>8</v>
       </c>
-      <c r="T21" s="27" t="s">
+      <c r="T21" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="25" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="10" t="s">
@@ -1894,22 +1894,22 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="P22" s="26">
+      <c r="P22" s="21">
         <v>9</v>
       </c>
-      <c r="Q22" s="27" t="s">
+      <c r="Q22" s="22" t="s">
         <v>36</v>
       </c>
       <c r="R22" s="1"/>
-      <c r="S22" s="26">
+      <c r="S22" s="21">
         <v>9</v>
       </c>
-      <c r="T22" s="27" t="s">
+      <c r="T22" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D23" s="11"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="10" t="s">
         <v>3</v>
       </c>
@@ -1921,26 +1921,26 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="P23" s="26">
+      <c r="P23" s="21">
         <v>10</v>
       </c>
-      <c r="Q23" s="27" t="s">
+      <c r="Q23" s="22" t="s">
         <v>62</v>
       </c>
       <c r="R23" s="1"/>
-      <c r="S23" s="26">
+      <c r="S23" s="21">
         <v>10</v>
       </c>
-      <c r="T23" s="27" t="s">
+      <c r="T23" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D24" s="11"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -1948,15 +1948,15 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="S24" s="29">
+      <c r="S24" s="24">
         <v>11</v>
       </c>
-      <c r="T24" s="27" t="s">
+      <c r="T24" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="25" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="10" t="s">
@@ -1965,287 +1965,297 @@
       <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
     </row>
     <row r="26" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D26" s="11"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D27" s="11"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="G27" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
     </row>
     <row r="29" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D29" s="19"/>
-      <c r="E29" s="16" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
     </row>
     <row r="30" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D30" s="19"/>
-      <c r="E30" s="16" t="s">
+      <c r="D30" s="28"/>
+      <c r="E30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
+      <c r="G30" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="18"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="15"/>
     </row>
     <row r="32" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D32" s="19"/>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
     </row>
     <row r="33" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D33" s="19"/>
-      <c r="E33" s="16" t="s">
+      <c r="D33" s="28"/>
+      <c r="E33" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
     </row>
     <row r="34" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D35" s="19"/>
-      <c r="E35" s="16" t="s">
+      <c r="D35" s="28"/>
+      <c r="E35" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
     </row>
     <row r="36" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D36" s="19"/>
-      <c r="E36" s="16" t="s">
+      <c r="D36" s="28"/>
+      <c r="E36" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
     </row>
     <row r="37" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
     </row>
     <row r="38" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D38" s="19"/>
-      <c r="E38" s="16" t="s">
+      <c r="D38" s="28"/>
+      <c r="E38" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
     </row>
     <row r="39" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D39" s="19"/>
-      <c r="E39" s="16" t="s">
+      <c r="D39" s="28"/>
+      <c r="E39" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
     </row>
     <row r="40" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
     </row>
     <row r="41" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D41" s="19"/>
-      <c r="E41" s="16" t="s">
+      <c r="D41" s="28"/>
+      <c r="E41" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
     </row>
     <row r="42" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D42" s="19"/>
-      <c r="E42" s="16" t="s">
+      <c r="D42" s="28"/>
+      <c r="E42" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F21:M21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="F16:M16"/>
+    <mergeCell ref="F17:M17"/>
+    <mergeCell ref="F18:M18"/>
     <mergeCell ref="D40:D42"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="S13:T13"/>
@@ -2262,16 +2272,6 @@
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="F19:M19"/>
     <mergeCell ref="F20:M20"/>
-    <mergeCell ref="F21:M21"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D8:M8"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="F16:M16"/>
-    <mergeCell ref="F17:M17"/>
-    <mergeCell ref="F18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>